<commit_message>
Követelmény Specifikáció : Vágyálom rendszer megírva
</commit_message>
<xml_diff>
--- a/KépernyőTervek.xlsx
+++ b/KépernyőTervek.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Vajda Krisztián\team4_afp1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\team4_afp1\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62432459-F5A0-4CEE-ACEA-B22F6C838E31}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KépernyőTervek" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>profilkép</t>
   </si>
@@ -42,11 +43,17 @@
   <si>
     <t>X</t>
   </si>
+  <si>
+    <t>Bejelentkezés</t>
+  </si>
+  <si>
+    <t>Regisztráció</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -231,28 +238,55 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -260,46 +294,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -336,7 +349,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Kép 1" descr="Check Correct Mark · Free vector graphic on Pixabay"/>
+        <xdr:cNvPr id="2" name="Kép 1" descr="Check Correct Mark · Free vector graphic on Pixabay">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -630,204 +649,352 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection sqref="A1:I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="2"/>
-    </row>
-    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="4"/>
-    </row>
-    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="10" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="12"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="4"/>
+    </row>
+    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="13"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="6"/>
+    </row>
+    <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
+      <c r="B3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="11" t="s">
+      <c r="C3" s="25"/>
+      <c r="D3" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="12"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="10" t="s">
+      <c r="E3" s="20"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="19"/>
-      <c r="I3" s="4"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="4"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="4"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="4"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="4"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="4"/>
-      <c r="L8" s="23"/>
-    </row>
-    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="4"/>
-    </row>
-    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="18" t="s">
+      <c r="H3" s="5"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="6"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="6"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="6"/>
+    </row>
+    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="13"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="6"/>
+    </row>
+    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="13"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="N7" s="11"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="6"/>
+    </row>
+    <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="13"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="N8" s="11"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="6"/>
+    </row>
+    <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="13"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="6"/>
+    </row>
+    <row r="10" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="13"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="17"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="4"/>
-    </row>
-    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="4"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="11" t="s">
+      <c r="E10" s="1"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="6"/>
+    </row>
+    <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="13"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="6"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="4"/>
-    </row>
-    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="4"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="4"/>
-    </row>
-    <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="5"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="6"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="6"/>
+    </row>
+    <row r="13" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="13"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="6"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="13"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="6"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="13"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="6"/>
+    </row>
+    <row r="16" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="14"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="19">
+    <mergeCell ref="J1:L16"/>
     <mergeCell ref="A1:A16"/>
     <mergeCell ref="H1:I16"/>
     <mergeCell ref="B1:G2"/>
@@ -841,6 +1008,11 @@
     <mergeCell ref="D12:E13"/>
     <mergeCell ref="D3:E9"/>
     <mergeCell ref="C3:C10"/>
+    <mergeCell ref="O1:R16"/>
+    <mergeCell ref="M1:N6"/>
+    <mergeCell ref="M9:N16"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="M8:N8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>